<commit_message>
Atualizando o Backlog (Chat)
</commit_message>
<xml_diff>
--- a/Documentacao do Projeto/Backlog Projeto.xlsx
+++ b/Documentacao do Projeto/Backlog Projeto.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Desktop\Faculdade\!projeto-individual\Projeto-Filme-Veio\Documentacao do Projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brufe\OneDrive\Área de Trabalho\Git\Projeto-Filme-Veio\Documentacao do Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1227B37C-F80A-46E9-8BFA-1422BABF1DFB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDF126F8-7857-4099-8380-1CA197E12E77}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="330" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="30">
   <si>
     <r>
       <t>§</t>
@@ -465,6 +465,41 @@
   </si>
   <si>
     <t>BACKLOG DO PROJETO</t>
+  </si>
+  <si>
+    <r>
+      <t>§</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Chat: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Local onde teremos o chat que será uma conversa entre os usuarios.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1104,21 +1139,84 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="25" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1128,71 +1226,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1598,7 +1633,7 @@
   <dimension ref="B1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="96" zoomScaleNormal="96" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:D21"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1611,149 +1646,149 @@
   <sheetData>
     <row r="1" spans="3:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="3:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
     </row>
     <row r="3" spans="3:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="41"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="43"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="35"/>
     </row>
     <row r="4" spans="3:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="44" t="s">
+      <c r="C4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="E4" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="44" t="s">
+      <c r="F4" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="46" t="s">
+      <c r="G4" s="37" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" spans="3:7" ht="20.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C5" s="45"/>
+      <c r="C5" s="48"/>
       <c r="D5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="44"/>
-      <c r="F5" s="44"/>
-      <c r="G5" s="46"/>
+      <c r="E5" s="36"/>
+      <c r="F5" s="36"/>
+      <c r="G5" s="37"/>
     </row>
     <row r="6" spans="3:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="20">
         <v>5</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="20">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C7" s="27">
+      <c r="C7" s="47">
         <v>2</v>
       </c>
-      <c r="D7" s="32" t="s">
+      <c r="D7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E7" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="42">
         <v>21</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="42">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="27"/>
-      <c r="D8" s="47" t="s">
+      <c r="C8" s="47"/>
+      <c r="D8" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
+      <c r="G8" s="43"/>
     </row>
     <row r="9" spans="3:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="27"/>
-      <c r="D9" s="47" t="s">
+      <c r="C9" s="47"/>
+      <c r="D9" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
+      <c r="G9" s="43"/>
     </row>
     <row r="10" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="27"/>
-      <c r="D10" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="29"/>
-      <c r="G10" s="29"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
+      <c r="G10" s="43"/>
     </row>
     <row r="11" spans="3:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="27"/>
-      <c r="D11" s="47" t="s">
+      <c r="C11" s="47"/>
+      <c r="D11" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="29"/>
-      <c r="G11" s="29"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
+      <c r="G11" s="43"/>
     </row>
     <row r="12" spans="3:7" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="27"/>
-      <c r="D12" s="47" t="s">
+      <c r="C12" s="47"/>
+      <c r="D12" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
+      <c r="G12" s="43"/>
     </row>
     <row r="13" spans="3:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="27"/>
-      <c r="D13" s="47" t="s">
+      <c r="C13" s="47"/>
+      <c r="D13" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="E13" s="30"/>
-      <c r="F13" s="30"/>
-      <c r="G13" s="30"/>
+      <c r="E13" s="44"/>
+      <c r="F13" s="44"/>
+      <c r="G13" s="44"/>
     </row>
     <row r="14" spans="3:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C14" s="13">
         <v>3</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="26" t="s">
+      <c r="E14" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="26">
+      <c r="F14" s="20">
         <v>13</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="20">
         <v>5</v>
       </c>
     </row>
@@ -1761,16 +1796,16 @@
       <c r="C15" s="13">
         <v>4</v>
       </c>
-      <c r="D15" s="33" t="s">
+      <c r="D15" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="26" t="s">
+      <c r="E15" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="20">
         <v>13</v>
       </c>
-      <c r="G15" s="26">
+      <c r="G15" s="20">
         <v>7</v>
       </c>
     </row>
@@ -1778,16 +1813,16 @@
       <c r="C16" s="11">
         <v>5</v>
       </c>
-      <c r="D16" s="33" t="s">
+      <c r="D16" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E16" s="26" t="s">
+      <c r="E16" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="20">
         <v>8</v>
       </c>
-      <c r="G16" s="26">
+      <c r="G16" s="20">
         <v>8</v>
       </c>
     </row>
@@ -1796,100 +1831,100 @@
       <c r="D17" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="19"/>
     </row>
     <row r="18" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B18" s="36"/>
-      <c r="C18" s="24">
+      <c r="B18" s="26"/>
+      <c r="C18" s="45">
         <v>6</v>
       </c>
-      <c r="D18" s="34" t="s">
+      <c r="D18" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="28">
+      <c r="F18" s="42">
         <v>13</v>
       </c>
-      <c r="G18" s="28">
+      <c r="G18" s="42">
         <v>3</v>
       </c>
     </row>
     <row r="19" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="36"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="48" t="s">
+      <c r="B19" s="26"/>
+      <c r="C19" s="46"/>
+      <c r="D19" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
     </row>
     <row r="20" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="36"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="48" t="s">
+      <c r="B20" s="26"/>
+      <c r="C20" s="46"/>
+      <c r="D20" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="29"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="29"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
     </row>
     <row r="21" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="36"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="48" t="s">
+      <c r="B21" s="26"/>
+      <c r="C21" s="46"/>
+      <c r="D21" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="30"/>
-      <c r="F21" s="30"/>
-      <c r="G21" s="30"/>
+      <c r="E21" s="44"/>
+      <c r="F21" s="44"/>
+      <c r="G21" s="44"/>
     </row>
     <row r="22" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="36"/>
-      <c r="C22" s="26">
+      <c r="B22" s="26"/>
+      <c r="C22" s="20">
         <v>7</v>
       </c>
-      <c r="D22" s="34" t="s">
+      <c r="D22" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="20">
         <v>8</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="20">
         <v>4</v>
       </c>
     </row>
     <row r="23" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="36"/>
+      <c r="B23" s="26"/>
       <c r="C23" s="12">
         <v>8</v>
       </c>
-      <c r="D23" s="35" t="s">
+      <c r="D23" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E23" s="26" t="s">
+      <c r="E23" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="20">
         <v>21</v>
       </c>
-      <c r="G23" s="26">
+      <c r="G23" s="20">
         <v>6</v>
       </c>
     </row>
     <row r="24" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="22"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="23"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="39"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -1909,5 +1944,6 @@
     <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>